<commit_message>
Modified Template and Picture features
</commit_message>
<xml_diff>
--- a/template-with-photo.xlsx
+++ b/template-with-photo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -22,16 +22,19 @@
     <t>First_Name</t>
   </si>
   <si>
+    <t>Parent ID</t>
+  </si>
+  <si>
+    <t>Manager_Name</t>
+  </si>
+  <si>
     <t>Designation</t>
   </si>
   <si>
-    <t>Parent ID</t>
+    <t>Photo</t>
   </si>
   <si>
     <t>Department</t>
-  </si>
-  <si>
-    <t>Photo</t>
   </si>
 </sst>
 </file>
@@ -44,7 +47,7 @@
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,10 +58,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -399,27 +408,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -525,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -543,140 +537,141 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -996,13 +991,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="14.8181818181818" customWidth="1"/>
@@ -1011,7 +1006,7 @@
     <col min="5" max="5" width="12.0909090909091" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1016,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1030,6 +1025,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>